<commit_message>
Update: Cambios en validaciones de CURP y como insertar en RPLocal
</commit_message>
<xml_diff>
--- a/public/archivos/PlantillaParaPadron.xlsx
+++ b/public/archivos/PlantillaParaPadron.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diegolopez/Documents/GitProyect/vales/apivales/public/archivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469060A8-C1F6-094C-A477-5AD314830161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35862903-E51E-3245-94C0-1A1926492EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{ED99B135-9311-0D4E-B87E-40D4C46CC0C6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Remesa</t>
   </si>
@@ -204,13 +204,22 @@
   </si>
   <si>
     <t>ESTATUS ORIGEN</t>
+  </si>
+  <si>
+    <t>CURP Anterior</t>
+  </si>
+  <si>
+    <t>Observacion en CURP</t>
+  </si>
+  <si>
+    <t>Identificador</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -219,25 +228,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri (Cuerpo)"/>
+    </font>
+    <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Calibri (Cuerpo)"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Calibri (Cuerpo)"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF002060"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Calibri (Cuerpo)"/>
     </font>
   </fonts>
   <fills count="10">
@@ -296,7 +307,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -362,52 +373,69 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -724,194 +752,206 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A9C34E-97D7-7B4E-8969-873A36362A97}">
-  <dimension ref="A3:BD4"/>
+  <dimension ref="A3:BG4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="9" ySplit="4" topLeftCell="J5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="4" topLeftCell="K5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="BA9" sqref="BA9"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="22.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="22.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.83203125" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="11" max="11" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" style="1" customWidth="1"/>
+    <col min="8" max="11" width="22.1640625" style="1"/>
+    <col min="12" max="12" width="3.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="22.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:56" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:56" ht="78" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="3" spans="1:59" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:59" ht="78" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="C4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="K4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="M4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="N4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="O4" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="P4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="Q4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="R4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="S4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="T4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="U4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="T4" s="2" t="s">
+      <c r="V4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="U4" s="2" t="s">
+      <c r="W4" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="V4" s="2" t="s">
+      <c r="X4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="Y4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="X4" s="8" t="s">
+      <c r="Z4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Y4" s="9" t="s">
+      <c r="AA4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="Z4" s="9" t="s">
+      <c r="AB4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="AA4" s="4" t="s">
+      <c r="AC4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="AB4" s="9" t="s">
+      <c r="AD4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="AC4" s="2" t="s">
+      <c r="AE4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AD4" s="4" t="s">
+      <c r="AF4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AE4" s="2" t="s">
+      <c r="AG4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AF4" s="2" t="s">
+      <c r="AH4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AG4" s="2" t="s">
+      <c r="AI4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AH4" s="7" t="s">
+      <c r="AJ4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="AI4" s="7" t="s">
+      <c r="AK4" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="AJ4" s="2" t="s">
+      <c r="AL4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AK4" s="4" t="s">
+      <c r="AM4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="AL4" s="4" t="s">
+      <c r="AN4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AM4" s="4" t="s">
+      <c r="AO4" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AN4" s="10" t="s">
+      <c r="AP4" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AO4" s="11" t="s">
+      <c r="AQ4" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="AP4" s="10" t="s">
+      <c r="AR4" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="AQ4" s="4" t="s">
+      <c r="AS4" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AR4" s="7" t="s">
+      <c r="AT4" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="AS4" s="7" t="s">
+      <c r="AU4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="AT4" s="7" t="s">
+      <c r="AV4" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="AU4" s="2" t="s">
+      <c r="AW4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AV4" s="2" t="s">
+      <c r="AX4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AW4" s="2" t="s">
+      <c r="AY4" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AX4" s="2" t="s">
+      <c r="AZ4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="AY4" s="2" t="s">
+      <c r="BA4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AZ4" s="2" t="s">
+      <c r="BB4" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="BA4" s="14" t="s">
+      <c r="BC4" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="BB4" s="14" t="s">
+      <c r="BD4" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="BC4" s="7" t="s">
+      <c r="BE4" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="BD4" s="12" t="s">
+      <c r="BF4" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="BG4" s="16" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update: Cambio en exportado de información de padrón, se agrega export
</commit_message>
<xml_diff>
--- a/public/archivos/PlantillaParaPadron.xlsx
+++ b/public/archivos/PlantillaParaPadron.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diegolopez/Documents/GitProyect/vales/apivales/public/archivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4447DD-D3EC-2B4F-884D-DD4FD96BF20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA0BD72-DE28-A04C-BC00-785CA383F367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{ED99B135-9311-0D4E-B87E-40D4C46CC0C6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Region_1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,17 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Remesa</t>
   </si>
   <si>
-    <t>Orden</t>
-  </si>
-  <si>
-    <t>Orden x mpio *</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -74,9 +68,6 @@
     <t>CURP *</t>
   </si>
   <si>
-    <t>Validador</t>
-  </si>
-  <si>
     <t>Municipio *</t>
   </si>
   <si>
@@ -116,58 +107,13 @@
     <t>FOLIO TARJETA GTO CONTIGO SÍ / IMPULSO</t>
   </si>
   <si>
-    <t>Apoyo_Solicitado *</t>
-  </si>
-  <si>
-    <t>Vertiente *</t>
-  </si>
-  <si>
     <t>Enlace / Origen *</t>
   </si>
   <si>
-    <t>Largo_CURP</t>
-  </si>
-  <si>
-    <t>Frecuencia_CURP</t>
-  </si>
-  <si>
-    <t>PERIODO</t>
-  </si>
-  <si>
-    <t>Nombres del menor*</t>
-  </si>
-  <si>
-    <t>Apellido_1 del menor*</t>
-  </si>
-  <si>
-    <t>Fecha_Nac_menor</t>
-  </si>
-  <si>
-    <t>Sexo_del_menor</t>
-  </si>
-  <si>
-    <t>Edo_Nac_del menor</t>
-  </si>
-  <si>
-    <t>CURP_del menor*</t>
-  </si>
-  <si>
-    <t>Validador_CURP_del_menor</t>
-  </si>
-  <si>
-    <t>Largo_CURP_menor</t>
-  </si>
-  <si>
-    <t>Frecuencia_CURP_menor</t>
-  </si>
-  <si>
     <t>RESPONSABLE DE VALIDACION</t>
   </si>
   <si>
     <t>FECHA VALIDACION</t>
-  </si>
-  <si>
-    <t>Apellido_2 del menor*</t>
   </si>
   <si>
     <t>APOYO ANTERIOR</t>
@@ -377,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -406,12 +352,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -736,45 +676,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A9C34E-97D7-7B4E-8969-873A36362A97}">
-  <dimension ref="A3:BG4"/>
+  <dimension ref="A3:AO4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="8" ySplit="4" topLeftCell="I5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="4" topLeftCell="AE5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="AL8" sqref="AL8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="1" customWidth="1"/>
-    <col min="6" max="9" width="22.1640625" style="1"/>
-    <col min="10" max="10" width="3.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="52" width="22.1640625" style="1"/>
-    <col min="53" max="53" width="17.83203125" style="1" customWidth="1"/>
-    <col min="54" max="54" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="16384" width="22.1640625" style="1"/>
+    <col min="2" max="2" width="5.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="1" customWidth="1"/>
+    <col min="4" max="7" width="22.1640625" style="1"/>
+    <col min="8" max="8" width="3.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="34" width="22.1640625" style="1"/>
+    <col min="35" max="35" width="17.83203125" style="1" customWidth="1"/>
+    <col min="36" max="36" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="16384" width="22.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:59" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:59" ht="78" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:41" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -783,161 +721,107 @@
       <c r="G4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="7" t="s">
         <v>9</v>
       </c>
       <c r="K4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="M4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="N4" s="8" t="s">
+      <c r="N4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="O4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="7" t="s">
+      <c r="P4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="5" t="s">
+      <c r="T4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="U4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="S4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="V4" s="3" t="s">
+      <c r="V4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="W4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="X4" s="9" t="s">
+      <c r="X4" s="5" t="s">
         <v>19</v>
       </c>
       <c r="Y4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="Z4" s="10" t="s">
+      <c r="Z4" s="3" t="s">
         <v>21</v>
       </c>
       <c r="AA4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="AB4" s="10" t="s">
+      <c r="AB4" s="3" t="s">
         <v>23</v>
       </c>
       <c r="AC4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI4" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AK4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="AD4" s="5" t="s">
+      <c r="AL4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AM4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AF4" s="3" t="s">
+      <c r="AN4" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO4" s="13" t="s">
         <v>27</v>
-      </c>
-      <c r="AG4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="AH4" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="AI4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="AK4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AL4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AM4" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="AN4" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="AO4" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="AP4" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="AQ4" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="AR4" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="AS4" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="AT4" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="AU4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AV4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AW4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="AX4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AY4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AZ4" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="BA4" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="BB4" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="BC4" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="BD4" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="BE4" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="BF4" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="BG4" s="15" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>